<commit_message>
Added all tests and checked in matlab
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\totna\Dokumentumok\Jupyter\Jump_Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B7EB05-C2A5-4B4A-BC4E-27227DFF99A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6F553F-DAF4-49B7-BDB0-2BDE59D9A3F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t>Test Name</t>
   </si>
@@ -82,6 +82,18 @@
   </si>
   <si>
     <t>LM</t>
+  </si>
+  <si>
+    <t>Variance swap</t>
+  </si>
+  <si>
+    <t>JO</t>
+  </si>
+  <si>
+    <t>Matches with original ML code?</t>
+  </si>
+  <si>
+    <t>Needs checking</t>
   </si>
 </sst>
 </file>
@@ -129,7 +141,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -149,36 +161,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="dashed">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dashed">
-        <color auto="1"/>
-      </left>
-      <right style="dashed">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="dashed">
         <color auto="1"/>
       </left>
@@ -237,13 +219,141 @@
         <color auto="1"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -251,22 +361,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -275,16 +388,40 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -394,8 +531,8 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>412750</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -410,8 +547,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7962900" y="1879600"/>
-          <a:ext cx="3714750" cy="692150"/>
+          <a:off x="10033000" y="1873250"/>
+          <a:ext cx="3714750" cy="3073400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -456,6 +593,24 @@
             <a:rPr lang="hu-HU" sz="1800" baseline="0"/>
             <a:t> PZ2 - What Tau was used by Maneesoonthorn?</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="hu-HU" sz="1800" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="hu-HU" sz="1800" baseline="0"/>
+            <a:t>With PZ, we use an other random (uniform) random variable - results are inconsistent</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="hu-HU" sz="1800" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="hu-HU" sz="1800" baseline="0"/>
+            <a:t>np.var in python and matlab "var" are different??? Manually set ddof in python</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -463,10 +618,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -732,10 +883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F13"/>
+  <dimension ref="B1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -746,181 +897,238 @@
     <col min="4" max="4" width="28.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="1"/>
+    <col min="7" max="7" width="27.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="3" t="s">
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="18" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B3" s="7" t="s">
+      <c r="G2" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="2">
-        <v>73</v>
-      </c>
-      <c r="F3" s="9">
+        <v>49</v>
+      </c>
+      <c r="F3" s="13">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="7" t="s">
+      <c r="G3" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="2">
-        <v>484</v>
-      </c>
-      <c r="F4" s="9">
+        <v>468</v>
+      </c>
+      <c r="F4" s="13">
         <v>464</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="7" t="s">
+      <c r="G4" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="2">
-        <v>53</v>
-      </c>
-      <c r="F5" s="9">
+        <v>35</v>
+      </c>
+      <c r="F5" s="13">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="7" t="s">
+      <c r="G5" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="2">
-        <v>59</v>
-      </c>
-      <c r="F6" s="9">
+        <v>56</v>
+      </c>
+      <c r="F6" s="13">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="10" t="s">
+      <c r="G6" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="11">
-        <v>119</v>
-      </c>
-      <c r="F7" s="12">
+      <c r="E7" s="6"/>
+      <c r="F7" s="14">
         <v>92</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B8" s="7" t="s">
+      <c r="G7" s="23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="2">
-        <v>116</v>
-      </c>
-      <c r="F8" s="9">
+      <c r="E8" s="2"/>
+      <c r="F8" s="13">
         <v>78</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="7" t="s">
+      <c r="G8" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="10" t="s">
+      <c r="G9" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="7" t="s">
+      <c r="D10" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="6">
+        <v>47</v>
+      </c>
+      <c r="F10" s="14">
+        <v>63</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="9"/>
-    </row>
-    <row r="12" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B13" s="7"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="11">
+        <v>90</v>
+      </c>
+      <c r="F12" s="15">
+        <v>79</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
       <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D6">

</xml_diff>